<commit_message>
Fitur Administrasi (Error Belum Fix)
</commit_message>
<xml_diff>
--- a/public/DataFile/administrasi_file.xlsx
+++ b/public/DataFile/administrasi_file.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/atmajabagastia/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D23E0AC-7B92-4443-A8F7-020820ACC982}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93CD0626-6CE5-3A40-AE3C-F7B74F41304D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="12460" xr2:uid="{59B4EBEB-453F-4BAB-BC88-D872411C6BD4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>No</t>
   </si>
@@ -33,13 +33,16 @@
     <t>Nama File</t>
   </si>
   <si>
-    <t>SP2D</t>
-  </si>
-  <si>
-    <t>SPM</t>
-  </si>
-  <si>
-    <t>SPBY</t>
+    <t>SP1</t>
+  </si>
+  <si>
+    <t>SP2</t>
+  </si>
+  <si>
+    <t>SP3</t>
+  </si>
+  <si>
+    <t>SP4</t>
   </si>
 </sst>
 </file>
@@ -391,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA0BEAEE-463E-4255-AF33-1A6A270DCB7B}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="138" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -431,6 +434,14 @@
         <v>4</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>